<commit_message>
change: data in voucher, tutor_application, teaching_style, subject, bill
</commit_message>
<xml_diff>
--- a/Dataset/bill.xlsx
+++ b/Dataset/bill.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>bill_id</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Xac nhan</t>
   </si>
   <si>
-    <t>Da hoan</t>
-  </si>
-  <si>
-    <t>Chua hoan</t>
-  </si>
-  <si>
     <t>Chua xac nhan</t>
   </si>
   <si>
@@ -58,6 +52,9 @@
   </si>
   <si>
     <t>Dong coc</t>
+  </si>
+  <si>
+    <t>Hoan coc</t>
   </si>
 </sst>
 </file>
@@ -459,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,8 +465,8 @@
     <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -509,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
@@ -527,10 +524,10 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3">
         <v>10</v>
@@ -546,17 +543,15 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3">
         <v>9</v>
       </c>
-      <c r="G4" s="3">
-        <v>3</v>
-      </c>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
@@ -570,7 +565,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3">
         <v>10</v>
@@ -589,7 +584,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" s="3">
         <v>8</v>
@@ -610,7 +605,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7" s="3">
         <v>11</v>
@@ -626,17 +621,15 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3">
         <v>12</v>
       </c>
-      <c r="G8" s="3">
-        <v>7</v>
-      </c>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
@@ -647,10 +640,10 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F9" s="3">
         <v>9</v>
@@ -666,10 +659,10 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="3">
         <v>12</v>
@@ -685,10 +678,10 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3">
         <v>11</v>

</xml_diff>